<commit_message>
Data of Project 3
</commit_message>
<xml_diff>
--- a/Data_Overview_Project3.xlsx
+++ b/Data_Overview_Project3.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -195,12 +195,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -541,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97B67AFA-570D-499C-BDAC-C53FE7A2D5BD}">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9:K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1011,10 +1010,10 @@
       <c r="I10">
         <v>0.1321389</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10">
         <v>1.008869</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10">
         <v>3.6442889999999999E-2</v>
       </c>
       <c r="L10">
@@ -1055,10 +1054,10 @@
       <c r="I11">
         <v>6.6319039999999996E-2</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11">
         <v>0.88544069999999997</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11">
         <v>4.3322069999999997E-2</v>
       </c>
       <c r="L11">
@@ -1099,10 +1098,10 @@
       <c r="I12">
         <v>4.0831680000000002E-2</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12">
         <v>1.071556</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12">
         <v>2.2821080000000001E-2</v>
       </c>
       <c r="L12">
@@ -1143,10 +1142,10 @@
       <c r="I13">
         <v>0.67909129999999995</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13">
         <v>0.89420160000000004</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13">
         <v>3.483907E-2</v>
       </c>
       <c r="L13">

</xml_diff>